<commit_message>
Updated website wheel chair render picture
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Expense</t>
   </si>
@@ -93,13 +93,19 @@
     <t>Kinect Mount</t>
   </si>
   <si>
-    <t>Fasteners, odds and ends</t>
-  </si>
-  <si>
     <t>Total expenses (actual and expected) minus funding:</t>
   </si>
   <si>
-    <t>Parts for PCB, connectors</t>
+    <t>Sonar Customs</t>
+  </si>
+  <si>
+    <t>PCB Customs</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>Parts for PCB</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,7 +561,7 @@
         <v>18</v>
       </c>
       <c r="G3">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -575,16 +581,10 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>150</v>
+        <v>138.35</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4">
-        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
@@ -604,16 +604,10 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
@@ -662,20 +656,55 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>85.76</v>
+      </c>
+    </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4">
         <f>SUM(D3:D13)</f>
-        <v>515</v>
+        <v>674.11</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="4">
         <f>SUM(G3:G12)</f>
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>7</v>
@@ -687,11 +716,11 @@
     </row>
     <row r="18" spans="5:6">
       <c r="E18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18">
         <f>D15+G15-K15</f>
-        <v>240</v>
+        <v>241.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated budget (should be final)
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Expense</t>
   </si>
@@ -75,15 +75,9 @@
     <t>Display Board</t>
   </si>
   <si>
-    <t>Printing (Rowan)</t>
-  </si>
-  <si>
     <t>PCBs</t>
   </si>
   <si>
-    <t>USD, tax/duty TBD</t>
-  </si>
-  <si>
     <t>Sheet Metal</t>
   </si>
   <si>
@@ -106,6 +100,21 @@
   </si>
   <si>
     <t>Parts for PCB</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Rowan</t>
+  </si>
+  <si>
+    <t>Iain</t>
+  </si>
+  <si>
+    <t>Per Person</t>
+  </si>
+  <si>
+    <t>Refund</t>
   </si>
 </sst>
 </file>
@@ -484,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,16 +561,10 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>145</v>
+        <v>146.88999999999999</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>67</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -595,7 +598,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -604,10 +607,7 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>160</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>144.07</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
@@ -618,10 +618,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -632,19 +632,13 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -658,7 +652,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -669,26 +663,46 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>17.05</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
       </c>
       <c r="D11">
         <v>85.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -697,30 +711,81 @@
       </c>
       <c r="D15" s="4">
         <f>SUM(D3:D13)</f>
-        <v>674.11</v>
+        <v>720.76999999999987</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="4">
         <f>SUM(G3:G12)</f>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K15" s="3">
         <f>SUM(K3:K13)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="E18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F18">
         <f>D15+G15-K15</f>
-        <v>241.11</v>
+        <v>270.76999999999987</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19">
+        <f>F18/3</f>
+        <v>90.256666666666618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <f>D3+D5+D9+D10+D11</f>
+        <v>415.41999999999996</v>
+      </c>
+      <c r="C20">
+        <f>B20-F19</f>
+        <v>325.16333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <f>D6+D7+D12</f>
+        <v>147</v>
+      </c>
+      <c r="C21">
+        <f>B21-F19</f>
+        <v>56.743333333333382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <f>D4+D8</f>
+        <v>158.35</v>
+      </c>
+      <c r="C22">
+        <f>B22-F19</f>
+        <v>68.093333333333376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to final report
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Expense</t>
   </si>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,12 +787,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>146.88999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>138.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>144.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>21.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>17.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>85.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <f>SUM(B3:B12)</f>
+        <v>720.76999999999987</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>